<commit_message>
preparing for migration to React frontend
</commit_message>
<xml_diff>
--- a/fields.xlsx
+++ b/fields.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="163">
   <si>
     <t>id</t>
   </si>
@@ -484,6 +484,27 @@
   </si>
   <si>
     <t>.id ',</t>
+  </si>
+  <si>
+    <t>d64</t>
+  </si>
+  <si>
+    <t>dwdynamic</t>
+  </si>
+  <si>
+    <t>dwdynamicdetails</t>
+  </si>
+  <si>
+    <t>(IF(dialysis_cards.pre_weight IS NULL OR dialysis_cards.dry_weight IS NULL, NULL, (dialysis_cards.pre_weight - dialysis_cards.dry_weight)*1000))</t>
+  </si>
+  <si>
+    <t>(dialysis_cards.dry_weight - t.dry_weight)</t>
+  </si>
+  <si>
+    <t>CONCAT(dialysis_cards.dry_weight,"_","(",DATE_FORMAT(dialysis_cards.date, "%d.%m.%Y"),")"," -- ",t.dry_weight,"_","(",DATE_FORMAT(t.date, "%d.%m.%Y"),")")</t>
+  </si>
+  <si>
+    <t>0 or 1</t>
   </si>
 </sst>
 </file>
@@ -500,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,6 +558,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -550,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -559,6 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -860,16 +888,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" activeCellId="3" sqref="C29 C28 C26 C25"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1097,6 +1126,9 @@
         <v>30</v>
       </c>
       <c r="C25" s="7"/>
+      <c r="D25" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1106,6 +1138,9 @@
         <v>32</v>
       </c>
       <c r="C26" s="7"/>
+      <c r="D26" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1129,6 +1164,9 @@
         <v>33</v>
       </c>
       <c r="C28" s="7"/>
+      <c r="D28" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1138,6 +1176,9 @@
         <v>34</v>
       </c>
       <c r="C29" s="7"/>
+      <c r="D29" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1311,6 +1352,9 @@
         <v>57</v>
       </c>
       <c r="C46" s="7"/>
+      <c r="D46" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1432,6 +1476,9 @@
         <v>59</v>
       </c>
       <c r="C61" s="7"/>
+      <c r="D61" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -1455,6 +1502,9 @@
         <v>61</v>
       </c>
       <c r="C63" s="7"/>
+      <c r="D63" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -1464,6 +1514,9 @@
         <v>62</v>
       </c>
       <c r="C64" s="7"/>
+      <c r="D64" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -1490,12 +1543,36 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
+      <c r="A68" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="2" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>